<commit_message>
download excel feature back onlinegit add .
</commit_message>
<xml_diff>
--- a/Dashboard/media/blr.xlsx
+++ b/Dashboard/media/blr.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\__gitam__\DashBoard-BackEnd\Dashboard\media\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2086783F-107D-4D45-ADFA-9F21F4186C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="CF 2022" sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
     <sheet name="SoT 2019" sheetId="13" state="hidden" r:id="rId4"/>
     <sheet name="GSBB 2019" sheetId="14" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,9 +39,6 @@
   </si>
   <si>
     <t>Bengaluru Campus</t>
-  </si>
-  <si>
-    <t>GSBB</t>
   </si>
   <si>
     <t>Total</t>
@@ -173,16 +164,19 @@
     <t>School of Business , Bengaluru - List of Corporates - UG - 2019</t>
   </si>
   <si>
-    <t>SoTB</t>
+    <t>GST</t>
   </si>
   <si>
-    <t>SoSB</t>
+    <t>GSS</t>
+  </si>
+  <si>
+    <t>GSB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15">
     <font>
       <sz val="10"/>
@@ -617,7 +611,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,12 +630,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,28 +742,28 @@
     </dxf>
   </dxfs>
   <tableStyles count="6">
-    <tableStyle name="SoT 2022 UG-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="SoT 2022 UG-style" pivot="0" count="2">
       <tableStyleElement type="firstRowStripe" dxfId="12"/>
       <tableStyleElement type="secondRowStripe" dxfId="11"/>
     </tableStyle>
-    <tableStyle name="SoT 2020-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="SoT 2020-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="10"/>
       <tableStyleElement type="firstRowStripe" dxfId="9"/>
       <tableStyleElement type="secondRowStripe" dxfId="8"/>
     </tableStyle>
-    <tableStyle name="GSBB 2020-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+    <tableStyle name="GSBB 2020-style" pivot="0" count="2">
       <tableStyleElement type="firstRowStripe" dxfId="7"/>
       <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
-    <tableStyle name="GSBB 2020-style 2" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
+    <tableStyle name="GSBB 2020-style 2" pivot="0" count="2">
       <tableStyleElement type="firstRowStripe" dxfId="5"/>
       <tableStyleElement type="secondRowStripe" dxfId="4"/>
     </tableStyle>
-    <tableStyle name="SoT 2019-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
+    <tableStyle name="SoT 2019-style" pivot="0" count="2">
       <tableStyleElement type="firstRowStripe" dxfId="3"/>
       <tableStyleElement type="secondRowStripe" dxfId="2"/>
     </tableStyle>
-    <tableStyle name="GSBB 2019-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
+    <tableStyle name="GSBB 2019-style" pivot="0" count="2">
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
@@ -786,36 +780,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A4:AB91" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A4:AB91" headerRowCount="0">
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Column7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Column10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Column11"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Column12"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Column13"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Column14"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Column15"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Column16"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Column17"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Column18"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Column19"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Column20"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Column21"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Column22"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="Column23"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Column24"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Column25"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="Column26"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Column27"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="Column28"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
+    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="9" name="Column9"/>
+    <tableColumn id="10" name="Column10"/>
+    <tableColumn id="11" name="Column11"/>
+    <tableColumn id="12" name="Column12"/>
+    <tableColumn id="13" name="Column13"/>
+    <tableColumn id="14" name="Column14"/>
+    <tableColumn id="15" name="Column15"/>
+    <tableColumn id="16" name="Column16"/>
+    <tableColumn id="17" name="Column17"/>
+    <tableColumn id="18" name="Column18"/>
+    <tableColumn id="19" name="Column19"/>
+    <tableColumn id="20" name="Column20"/>
+    <tableColumn id="21" name="Column21"/>
+    <tableColumn id="22" name="Column22"/>
+    <tableColumn id="23" name="Column23"/>
+    <tableColumn id="24" name="Column24"/>
+    <tableColumn id="25" name="Column25"/>
+    <tableColumn id="26" name="Column26"/>
+    <tableColumn id="27" name="Column27"/>
+    <tableColumn id="28" name="Column28"/>
   </tableColumns>
   <tableStyleInfo name="SoT 2020-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -827,75 +821,75 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="H4:AA24" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table_3" displayName="Table_3" ref="H4:AA24" headerRowCount="0">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Column7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Column10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Column11"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Column12"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Column13"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Column14"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Column15"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Column16"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Column17"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Column18"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Column19"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Column20"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
+    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="9" name="Column9"/>
+    <tableColumn id="10" name="Column10"/>
+    <tableColumn id="11" name="Column11"/>
+    <tableColumn id="12" name="Column12"/>
+    <tableColumn id="13" name="Column13"/>
+    <tableColumn id="14" name="Column14"/>
+    <tableColumn id="15" name="Column15"/>
+    <tableColumn id="16" name="Column16"/>
+    <tableColumn id="17" name="Column17"/>
+    <tableColumn id="18" name="Column18"/>
+    <tableColumn id="19" name="Column19"/>
+    <tableColumn id="20" name="Column20"/>
   </tableColumns>
   <tableStyleInfo name="GSBB 2020-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A4:F33" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table_4" displayName="Table_4" ref="A4:F33" headerRowCount="0">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Column6"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
   </tableColumns>
   <tableStyleInfo name="GSBB 2020-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A4:K57" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table_5" displayName="Table_5" ref="A4:K57" headerRowCount="0">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Column7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Column10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Column11"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
+    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="9" name="Column9"/>
+    <tableColumn id="10" name="Column10"/>
+    <tableColumn id="11" name="Column11"/>
   </tableColumns>
   <tableStyleInfo name="SoT 2019-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="A4:F36" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table_6" displayName="Table_6" ref="A4:F36" headerRowCount="0">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Column6"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
   </tableColumns>
   <tableStyleInfo name="GSBB 2019-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1098,7 +1092,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1106,8 +1100,8 @@
   <dimension ref="A1:J1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:H3"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1152,20 +1146,20 @@
     <row r="3" spans="1:10" ht="25.5" customHeight="1">
       <c r="A3" s="48"/>
       <c r="B3" s="48"/>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="57"/>
+      <c r="E3" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="62" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="63" t="s">
+      <c r="H3" s="55"/>
+      <c r="I3" s="59" t="s">
         <v>4</v>
-      </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="57" t="s">
-        <v>5</v>
       </c>
       <c r="J3" s="55"/>
     </row>
@@ -1173,28 +1167,28 @@
       <c r="A4" s="49"/>
       <c r="B4" s="49"/>
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1">
@@ -1202,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1224,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1246,7 +1240,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
@@ -1268,7 +1262,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1290,7 +1284,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1312,7 +1306,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1332,7 +1326,7 @@
     <row r="11" spans="1:10" ht="18.75" customHeight="1">
       <c r="A11" s="48"/>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1352,7 +1346,7 @@
     <row r="12" spans="1:10" ht="18.75" customHeight="1">
       <c r="A12" s="48"/>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1372,7 +1366,7 @@
     <row r="13" spans="1:10" ht="18.75" customHeight="1">
       <c r="A13" s="49"/>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1394,7 +1388,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1416,7 +1410,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1438,7 +1432,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1460,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1482,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1504,7 +1498,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1526,7 +1520,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1548,7 +1542,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1570,7 +1564,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1592,7 +1586,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1614,7 +1608,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1628,7 +1622,7 @@
     <row r="25" spans="1:10" ht="18.75" customHeight="1">
       <c r="A25" s="48"/>
       <c r="B25" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -1648,7 +1642,7 @@
     <row r="26" spans="1:10" ht="18.75" customHeight="1">
       <c r="A26" s="48"/>
       <c r="B26" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -1668,7 +1662,7 @@
     <row r="27" spans="1:10" ht="18.75" customHeight="1">
       <c r="A27" s="49"/>
       <c r="B27" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -4630,7 +4624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -4656,7 +4650,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75">
-      <c r="A1" s="58" t="str">
+      <c r="A1" s="60" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("importrange(""1mGGGnROFWKpKE3zvFsTFyea9Hgzwwcuu-BICnewevT4"",""UR!A:aa"")"),"#REF!")</f>
         <v>#REF!</v>
       </c>
@@ -4688,7 +4682,7 @@
       <c r="AA1" s="52"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A2" s="59"/>
+      <c r="A2" s="61"/>
       <c r="B2" s="54"/>
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
@@ -4717,7 +4711,7 @@
       <c r="AA2" s="55"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A3" s="59"/>
+      <c r="A3" s="61"/>
       <c r="B3" s="54"/>
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
@@ -11969,7 +11963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -41008,7 +41002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -41041,8 +41035,8 @@
       <c r="K1" s="33"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="60" t="s">
-        <v>36</v>
+      <c r="A2" s="62" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="54"/>
@@ -41054,8 +41048,8 @@
       <c r="I2" s="54"/>
       <c r="J2" s="54"/>
       <c r="K2" s="55"/>
-      <c r="L2" s="61" t="s">
-        <v>37</v>
+      <c r="L2" s="63" t="s">
+        <v>36</v>
       </c>
       <c r="M2" s="54"/>
       <c r="N2" s="54"/>
@@ -41068,54 +41062,54 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="E3" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="35" t="s">
-        <v>34</v>
+      <c r="F3" s="34" t="s">
+        <v>37</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="G3" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="H3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="I3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="J3" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="K3" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="34" t="s">
-        <v>43</v>
+      <c r="L3" s="36" t="s">
+        <v>30</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="M3" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="N3" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="36" t="s">
+      <c r="O3" s="36" t="s">
         <v>33</v>
-      </c>
-      <c r="O3" s="36" t="s">
-        <v>34</v>
       </c>
       <c r="P3" s="36"/>
       <c r="Q3" s="36"/>
       <c r="R3" s="36"/>
       <c r="S3" s="36"/>
       <c r="T3" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="12.75">
@@ -50472,7 +50466,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -50508,16 +50502,16 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="60" t="s">
-        <v>44</v>
+      <c r="A2" s="62" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
       <c r="E2" s="54"/>
       <c r="F2" s="55"/>
-      <c r="H2" s="61" t="s">
-        <v>45</v>
+      <c r="H2" s="63" t="s">
+        <v>44</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="54"/>
@@ -50527,36 +50521,36 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="E3" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="34" t="s">
-        <v>34</v>
-      </c>
       <c r="F3" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="36"/>
       <c r="J3" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="L3" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="M3" s="36" t="s">
         <v>34</v>
-      </c>
-      <c r="M3" s="36" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="12.75">

</xml_diff>